<commit_message>
I've clearly waited too long to do this
</commit_message>
<xml_diff>
--- a/_analysis/Depth-Mapping/_dat/LevelLoggers/Logger Summary.xlsx
+++ b/_analysis/Depth-Mapping/_dat/LevelLoggers/Logger Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victoria Starnes\Documents\GitHub\Bluff-Lake-Project\_analysis\Depth-Mapping\_dat\LevelLoggers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BBE41A-85CC-43EF-BFFD-734D32F71A45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47E50A0-DC8B-4139-AD19-04925F32D91F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C64EC215-6CE1-46CD-BAD1-2EACF9D70C3A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Sonde Number</t>
   </si>
@@ -510,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A70250-E807-4561-B782-4439B4849A41}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,6 +917,61 @@
         <v>17</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43592</v>
+      </c>
+      <c r="B21">
+        <v>20089579</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>0.2</v>
+      </c>
+      <c r="I21">
+        <v>1.5</v>
+      </c>
+      <c r="J21">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>43684</v>
+      </c>
+      <c r="B22" s="3">
+        <v>10868630</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>